<commit_message>
Resources for Cancer knowledge panel
These resources are generated based on EXCEL files provided by Jeremy.
</commit_message>
<xml_diff>
--- a/resources/RNAvolume.xlsx
+++ b/resources/RNAvolume.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plateau/Documents/GitHub/PanoramiR/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFA975D-A686-3247-88B7-FEE14AA3A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE63EB4-E159-9D46-A7DB-54AD5435C33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3400" yWindow="2300" windowWidth="26840" windowHeight="15620" xr2:uid="{21F828FD-9FB1-3648-BBEB-1875B7C1153E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF5063B-D2D5-AC46-B51D-81EF87668391}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A12" sqref="A8:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,46 +456,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>